<commit_message>
Se corrige el activo H2-HO01-VE01
</commit_message>
<xml_diff>
--- a/DATOS-MOTORES-PLANTA.xlsx
+++ b/DATOS-MOTORES-PLANTA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1366DF-9883-48F4-BF40-0D61D538A87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF43501-9D55-4325-9DA0-D5A882543ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="636">
   <si>
     <t>Ubicación</t>
   </si>
@@ -2004,6 +2004,9 @@
   </si>
   <si>
     <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>H2-HO01-VE01-MT01</t>
   </si>
 </sst>
 </file>
@@ -4689,8 +4692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731214AF-4FD7-4F42-8356-E06FD5D5889D}">
   <dimension ref="A1:W86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5755,7 +5758,7 @@
     </row>
     <row r="16" spans="1:22" s="81" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="142" t="s">
-        <v>327</v>
+        <v>635</v>
       </c>
       <c r="B16" s="129" t="s">
         <v>482</v>
@@ -18924,6 +18927,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b8724930-3eb3-40b5-912f-63a542c79450" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008417DE73F65C1044A842071FF60F9C24" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2f7779624259339e165a6ddb578d532f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b8724930-3eb3-40b5-912f-63a542c79450" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9c1fe8137e1d498bcb24215ff06365a" ns3:_="">
     <xsd:import namespace="b8724930-3eb3-40b5-912f-63a542c79450"/>
@@ -19131,24 +19151,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59489610-4A72-41EB-ADD4-F523401201B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b8724930-3eb3-40b5-912f-63a542c79450"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b8724930-3eb3-40b5-912f-63a542c79450" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C06C305-4FFE-445C-A3E8-27E6924C4D5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFD598EE-C738-413D-B845-A6334C427961}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19164,28 +19191,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C06C305-4FFE-445C-A3E8-27E6924C4D5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59489610-4A72-41EB-ADD4-F523401201B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b8724930-3eb3-40b5-912f-63a542c79450"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>